<commit_message>
update lab worker comments
</commit_message>
<xml_diff>
--- a/Assignment 1/G1_Acceptance.Ass.1.xlsx
+++ b/Assignment 1/G1_Acceptance.Ass.1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16729"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="14640" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="462" windowWidth="25602" windowHeight="14640" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Names | Group 1" sheetId="8" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="601">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1070" uniqueCount="609">
   <si>
     <t xml:space="preserve">Use Case: </t>
   </si>
@@ -3441,6 +3441,30 @@
   <si>
     <t>In case  Manager want to view monthly report and System display successfully 
 the report.</t>
+  </si>
+  <si>
+    <t>Reference not in DB</t>
+  </si>
+  <si>
+    <t>Missing reference date</t>
+  </si>
+  <si>
+    <t>Missing client's ID</t>
+  </si>
+  <si>
+    <t>Missing specialist ID</t>
+  </si>
+  <si>
+    <t>Missing client's ID and Date</t>
+  </si>
+  <si>
+    <t>Missing client's Id and specialist ID</t>
+  </si>
+  <si>
+    <t>Missing date and specialist ID</t>
+  </si>
+  <si>
+    <t>Missing all required fields</t>
   </si>
 </sst>
 </file>
@@ -4296,9 +4320,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4344,24 +4365,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4376,6 +4397,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4800,7 +4824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I116"/>
   <sheetViews>
-    <sheetView topLeftCell="A111" workbookViewId="0">
+    <sheetView topLeftCell="A95" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -6201,10 +6225,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="155" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="157"/>
+      <c r="B1" s="156"/>
     </row>
     <row r="2" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A2" s="25" t="s">
@@ -6330,10 +6354,10 @@
     </row>
     <row r="16" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="156" t="s">
+      <c r="A17" s="155" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="157"/>
+      <c r="B17" s="156"/>
     </row>
     <row r="18" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A18" s="25" t="s">
@@ -6512,10 +6536,10 @@
       <c r="D34" s="71"/>
     </row>
     <row r="35" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="156" t="s">
+      <c r="A35" s="155" t="s">
         <v>69</v>
       </c>
-      <c r="B35" s="157"/>
+      <c r="B35" s="156"/>
     </row>
     <row r="36" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A36" s="25" t="s">
@@ -6654,10 +6678,10 @@
       <c r="D50" s="71"/>
     </row>
     <row r="51" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="156" t="s">
+      <c r="A51" s="155" t="s">
         <v>259</v>
       </c>
-      <c r="B51" s="157"/>
+      <c r="B51" s="156"/>
     </row>
     <row r="52" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A52" s="25" t="s">
@@ -6773,10 +6797,10 @@
     </row>
     <row r="65" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="66" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A66" s="156" t="s">
+      <c r="A66" s="155" t="s">
         <v>190</v>
       </c>
-      <c r="B66" s="157"/>
+      <c r="B66" s="156"/>
     </row>
     <row r="67" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A67" s="25" t="s">
@@ -6885,10 +6909,10 @@
     </row>
     <row r="79" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="80" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A80" s="156" t="s">
+      <c r="A80" s="155" t="s">
         <v>196</v>
       </c>
-      <c r="B80" s="157"/>
+      <c r="B80" s="156"/>
     </row>
     <row r="81" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A81" s="25" t="s">
@@ -6997,10 +7021,10 @@
     </row>
     <row r="93" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="94" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A94" s="156" t="s">
+      <c r="A94" s="155" t="s">
         <v>198</v>
       </c>
-      <c r="B94" s="157"/>
+      <c r="B94" s="156"/>
     </row>
     <row r="95" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A95" s="25" t="s">
@@ -7139,10 +7163,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="155" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="157"/>
+      <c r="B1" s="156"/>
     </row>
     <row r="2" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A2" s="25" t="s">
@@ -7181,16 +7205,16 @@
       </c>
     </row>
     <row r="8" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A8" s="152" t="s">
+      <c r="A8" s="151" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="152" t="s">
+      <c r="B8" s="151" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="152" t="s">
+      <c r="C8" s="151" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="152" t="s">
+      <c r="D8" s="151" t="s">
         <v>17</v>
       </c>
     </row>
@@ -7204,7 +7228,7 @@
       <c r="C9" s="115" t="s">
         <v>289</v>
       </c>
-      <c r="D9" s="153" t="s">
+      <c r="D9" s="152" t="s">
         <v>290</v>
       </c>
     </row>
@@ -7218,7 +7242,7 @@
       <c r="C10" s="117" t="s">
         <v>292</v>
       </c>
-      <c r="D10" s="154" t="s">
+      <c r="D10" s="153" t="s">
         <v>316</v>
       </c>
     </row>
@@ -7232,87 +7256,87 @@
       <c r="C11" s="117" t="s">
         <v>294</v>
       </c>
-      <c r="D11" s="150" t="s">
+      <c r="D11" s="149" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="83.4" x14ac:dyDescent="0.45">
-      <c r="A12" s="160" t="s">
+      <c r="A12" s="159" t="s">
         <v>296</v>
       </c>
       <c r="B12" s="117" t="s">
         <v>320</v>
       </c>
-      <c r="C12" s="150" t="s">
+      <c r="C12" s="149" t="s">
         <v>333</v>
       </c>
-      <c r="D12" s="159" t="s">
+      <c r="D12" s="158" t="s">
         <v>331</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="83.4" x14ac:dyDescent="0.45">
-      <c r="A13" s="161"/>
+      <c r="A13" s="160"/>
       <c r="B13" s="117" t="s">
         <v>297</v>
       </c>
       <c r="C13" s="117" t="s">
         <v>334</v>
       </c>
-      <c r="D13" s="159"/>
+      <c r="D13" s="158"/>
     </row>
     <row r="14" spans="1:4" ht="139.5" x14ac:dyDescent="0.45">
-      <c r="A14" s="161"/>
-      <c r="B14" s="150" t="s">
+      <c r="A14" s="160"/>
+      <c r="B14" s="149" t="s">
         <v>298</v>
       </c>
       <c r="C14" s="117" t="s">
         <v>336</v>
       </c>
-      <c r="D14" s="159"/>
+      <c r="D14" s="158"/>
     </row>
     <row r="15" spans="1:4" ht="83.4" x14ac:dyDescent="0.45">
-      <c r="A15" s="158" t="s">
+      <c r="A15" s="157" t="s">
         <v>337</v>
       </c>
       <c r="B15" s="117" t="s">
         <v>332</v>
       </c>
-      <c r="C15" s="150" t="s">
+      <c r="C15" s="149" t="s">
         <v>333</v>
       </c>
-      <c r="D15" s="159" t="s">
+      <c r="D15" s="158" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="97.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="158"/>
+      <c r="A16" s="157"/>
       <c r="B16" s="117" t="s">
         <v>300</v>
       </c>
       <c r="C16" s="117" t="s">
         <v>335</v>
       </c>
-      <c r="D16" s="159"/>
+      <c r="D16" s="158"/>
     </row>
     <row r="17" spans="1:4" ht="27.9" x14ac:dyDescent="0.45">
-      <c r="A17" s="158"/>
+      <c r="A17" s="157"/>
       <c r="B17" s="117" t="s">
         <v>301</v>
       </c>
-      <c r="C17" s="155" t="s">
+      <c r="C17" s="154" t="s">
         <v>302</v>
       </c>
-      <c r="D17" s="159"/>
+      <c r="D17" s="158"/>
     </row>
     <row r="18" spans="1:4" ht="72" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="158"/>
+      <c r="A18" s="157"/>
       <c r="B18" s="117" t="s">
         <v>303</v>
       </c>
-      <c r="C18" s="155" t="s">
+      <c r="C18" s="154" t="s">
         <v>304</v>
       </c>
-      <c r="D18" s="159"/>
+      <c r="D18" s="158"/>
     </row>
     <row r="19" spans="1:4" ht="56.1" x14ac:dyDescent="0.45">
       <c r="A19" s="137" t="s">
@@ -7398,10 +7422,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="155" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="157"/>
+      <c r="B1" s="156"/>
     </row>
     <row r="2" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A2" s="25" t="s">
@@ -7527,10 +7551,10 @@
     </row>
     <row r="16" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="17" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="164" t="s">
+      <c r="A17" s="161" t="s">
         <v>341</v>
       </c>
-      <c r="B17" s="165"/>
+      <c r="B17" s="162"/>
       <c r="C17" s="100"/>
       <c r="D17" s="100"/>
     </row>
@@ -7657,16 +7681,16 @@
       </c>
     </row>
     <row r="29" spans="1:4" ht="82.8" x14ac:dyDescent="0.45">
-      <c r="A29" s="147" t="s">
+      <c r="A29" s="146" t="s">
         <v>513</v>
       </c>
-      <c r="B29" s="148" t="s">
+      <c r="B29" s="147" t="s">
         <v>514</v>
       </c>
-      <c r="C29" s="148" t="s">
+      <c r="C29" s="147" t="s">
         <v>515</v>
       </c>
-      <c r="D29" s="149" t="s">
+      <c r="D29" s="148" t="s">
         <v>516</v>
       </c>
     </row>
@@ -7674,10 +7698,10 @@
       <c r="A30" s="138" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="150" t="s">
+      <c r="B30" s="149" t="s">
         <v>355</v>
       </c>
-      <c r="C30" s="151" t="s">
+      <c r="C30" s="150" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="118" t="s">
@@ -7686,10 +7710,10 @@
     </row>
     <row r="32" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="33" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="156" t="s">
+      <c r="A33" s="155" t="s">
         <v>345</v>
       </c>
-      <c r="B33" s="157"/>
+      <c r="B33" s="156"/>
     </row>
     <row r="34" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A34" s="25" t="s">
@@ -7787,10 +7811,10 @@
     </row>
     <row r="44" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="45" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="156" t="s">
+      <c r="A45" s="155" t="s">
         <v>449</v>
       </c>
-      <c r="B45" s="157"/>
+      <c r="B45" s="156"/>
     </row>
     <row r="46" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A46" s="25" t="s">
@@ -7896,10 +7920,10 @@
     </row>
     <row r="58" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="59" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A59" s="156" t="s">
+      <c r="A59" s="155" t="s">
         <v>459</v>
       </c>
-      <c r="B59" s="157"/>
+      <c r="B59" s="156"/>
     </row>
     <row r="60" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A60" s="25" t="s">
@@ -8033,10 +8057,10 @@
     </row>
     <row r="74" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="75" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A75" s="156" t="s">
+      <c r="A75" s="155" t="s">
         <v>478</v>
       </c>
-      <c r="B75" s="157"/>
+      <c r="B75" s="156"/>
     </row>
     <row r="76" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A76" s="25" t="s">
@@ -8158,10 +8182,10 @@
     </row>
     <row r="89" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="90" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A90" s="156" t="s">
+      <c r="A90" s="155" t="s">
         <v>518</v>
       </c>
-      <c r="B90" s="157"/>
+      <c r="B90" s="156"/>
     </row>
     <row r="91" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A91" s="25" t="s">
@@ -8267,10 +8291,10 @@
     </row>
     <row r="103" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="104" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A104" s="156" t="s">
+      <c r="A104" s="155" t="s">
         <v>528</v>
       </c>
-      <c r="B104" s="157"/>
+      <c r="B104" s="156"/>
     </row>
     <row r="105" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A105" s="25" t="s">
@@ -8372,10 +8396,10 @@
     </row>
     <row r="117" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="118" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A118" s="156" t="s">
+      <c r="A118" s="155" t="s">
         <v>538</v>
       </c>
-      <c r="B118" s="157"/>
+      <c r="B118" s="156"/>
     </row>
     <row r="119" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A119" s="25" t="s">
@@ -8459,10 +8483,10 @@
     </row>
     <row r="130" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="131" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A131" s="156" t="s">
+      <c r="A131" s="155" t="s">
         <v>547</v>
       </c>
-      <c r="B131" s="157"/>
+      <c r="B131" s="156"/>
     </row>
     <row r="132" spans="1:4" ht="14.1" x14ac:dyDescent="0.45">
       <c r="A132" s="25" t="s">
@@ -8566,8 +8590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView topLeftCell="A57" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="A49" sqref="A49:B49"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.80859375" defaultRowHeight="13.8" x14ac:dyDescent="0.45"/>
@@ -8579,10 +8603,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="166" t="s">
+      <c r="A1" s="163" t="s">
         <v>356</v>
       </c>
-      <c r="B1" s="167"/>
+      <c r="B1" s="164"/>
     </row>
     <row r="2" spans="1:4" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A2" s="139" t="s">
@@ -8661,7 +8685,7 @@
         <v>499</v>
       </c>
       <c r="D11" s="142" t="s">
-        <v>360</v>
+        <v>601</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="110.4" x14ac:dyDescent="0.45">
@@ -8675,7 +8699,7 @@
         <v>499</v>
       </c>
       <c r="D12" s="142" t="s">
-        <v>360</v>
+        <v>602</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="110.4" x14ac:dyDescent="0.45">
@@ -8689,7 +8713,7 @@
         <v>499</v>
       </c>
       <c r="D13" s="142" t="s">
-        <v>360</v>
+        <v>603</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="110.4" x14ac:dyDescent="0.45">
@@ -8703,7 +8727,7 @@
         <v>499</v>
       </c>
       <c r="D14" s="142" t="s">
-        <v>360</v>
+        <v>604</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="110.4" x14ac:dyDescent="0.45">
@@ -8717,7 +8741,7 @@
         <v>499</v>
       </c>
       <c r="D15" s="142" t="s">
-        <v>360</v>
+        <v>605</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="110.4" x14ac:dyDescent="0.45">
@@ -8731,7 +8755,7 @@
         <v>499</v>
       </c>
       <c r="D16" s="142" t="s">
-        <v>360</v>
+        <v>606</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="110.4" x14ac:dyDescent="0.45">
@@ -8745,7 +8769,7 @@
         <v>499</v>
       </c>
       <c r="D17" s="142" t="s">
-        <v>360</v>
+        <v>607</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="110.4" x14ac:dyDescent="0.45">
@@ -8759,7 +8783,7 @@
         <v>499</v>
       </c>
       <c r="D18" s="142" t="s">
-        <v>360</v>
+        <v>608</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="110.4" x14ac:dyDescent="0.45">
@@ -8772,16 +8796,16 @@
       <c r="C19" s="117" t="s">
         <v>499</v>
       </c>
-      <c r="D19" s="142" t="s">
-        <v>360</v>
+      <c r="D19" s="144" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="22" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A22" s="162" t="s">
+      <c r="A22" s="165" t="s">
         <v>362</v>
       </c>
-      <c r="B22" s="163"/>
+      <c r="B22" s="166"/>
     </row>
     <row r="23" spans="1:4" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A23" s="139" t="s">
@@ -8859,16 +8883,16 @@
       <c r="C32" s="145" t="s">
         <v>27</v>
       </c>
-      <c r="D32" s="146" t="s">
+      <c r="D32" s="172" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="35" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A35" s="156" t="s">
+      <c r="A35" s="155" t="s">
         <v>369</v>
       </c>
-      <c r="B35" s="157"/>
+      <c r="B35" s="156"/>
     </row>
     <row r="36" spans="1:4" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A36" s="139" t="s">
@@ -8980,10 +9004,10 @@
     </row>
     <row r="48" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="49" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A49" s="166" t="s">
+      <c r="A49" s="163" t="s">
         <v>379</v>
       </c>
-      <c r="B49" s="167"/>
+      <c r="B49" s="164"/>
     </row>
     <row r="50" spans="1:4" ht="14.1" x14ac:dyDescent="0.5">
       <c r="A50" s="139" t="s">
@@ -9107,10 +9131,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="168" t="s">
+      <c r="A1" s="167" t="s">
         <v>389</v>
       </c>
-      <c r="B1" s="169"/>
+      <c r="B1" s="168"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="87" t="s">
@@ -9191,10 +9215,10 @@
     </row>
     <row r="13" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="14" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="168" t="s">
+      <c r="A14" s="167" t="s">
         <v>399</v>
       </c>
-      <c r="B14" s="169"/>
+      <c r="B14" s="168"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" s="87" t="s">
@@ -9345,10 +9369,10 @@
     </row>
     <row r="32" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="33" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A33" s="168" t="s">
+      <c r="A33" s="167" t="s">
         <v>422</v>
       </c>
-      <c r="B33" s="169"/>
+      <c r="B33" s="168"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A34" s="87" t="s">
@@ -9511,7 +9535,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
@@ -9524,10 +9548,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="155" t="s">
         <v>574</v>
       </c>
-      <c r="B1" s="157"/>
+      <c r="B1" s="156"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" s="87" t="s">
@@ -9581,7 +9605,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="96.6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:4" ht="69" x14ac:dyDescent="0.45">
       <c r="A9" s="136" t="s">
         <v>576</v>
       </c>
@@ -9595,7 +9619,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="82.8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:4" ht="69" x14ac:dyDescent="0.45">
       <c r="A10" s="128" t="s">
         <v>577</v>
       </c>
@@ -9610,10 +9634,10 @@
       </c>
     </row>
     <row r="13" spans="1:4" ht="14.1" x14ac:dyDescent="0.5">
-      <c r="A13" s="170" t="s">
+      <c r="A13" s="169" t="s">
         <v>583</v>
       </c>
-      <c r="B13" s="170"/>
+      <c r="B13" s="169"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" s="66" t="s">
@@ -9697,10 +9721,10 @@
     </row>
     <row r="25" spans="1:4" ht="14.1" thickBot="1" x14ac:dyDescent="0.5"/>
     <row r="26" spans="1:4" ht="14.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A26" s="171" t="s">
+      <c r="A26" s="170" t="s">
         <v>593</v>
       </c>
-      <c r="B26" s="172"/>
+      <c r="B26" s="171"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A27" s="87" t="s">

</xml_diff>